<commit_message>
Upload Y4_B2526_General_Surgery_checklist1758123562297_backup@backdoor.com.xlsx via attendance app
</commit_message>
<xml_diff>
--- a/log_history/Y4_B2526_General_Surgery_checklist1758123562297_backup@backdoor.com.xlsx
+++ b/log_history/Y4_B2526_General_Surgery_checklist1758123562297_backup@backdoor.com.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham\Desktop\log_history\Imported_logs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham\Desktop\log_history\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2D99C0D-3EF2-4C8C-8ACF-EB5B8BDC7A4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A36E19AB-CDD1-47C4-9FB3-D134CE76B0FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="1300" windowWidth="18280" windowHeight="13100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1900" yWindow="1300" windowWidth="18280" windowHeight="13100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist" sheetId="1" r:id="rId1"/>
@@ -372,12 +372,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -403,10 +410,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -749,16 +757,16 @@
   <dimension ref="A1:F106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="D2" sqref="D2:D106"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="14.25" style="1" customWidth="1"/>
     <col min="4" max="4" width="13.6640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -778,7 +786,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -788,8 +796,8 @@
       <c r="C2" s="1">
         <v>45913</v>
       </c>
-      <c r="D2" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D2" s="3">
+        <v>0.46059027777777778</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
@@ -798,7 +806,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -808,8 +816,8 @@
       <c r="C3" s="1">
         <v>45913</v>
       </c>
-      <c r="D3" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D3" s="3">
+        <v>0.46059027777777778</v>
       </c>
       <c r="E3" t="s">
         <v>11</v>
@@ -818,7 +826,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -828,8 +836,8 @@
       <c r="C4" s="1">
         <v>45913</v>
       </c>
-      <c r="D4" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D4" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
@@ -838,7 +846,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -848,8 +856,8 @@
       <c r="C5" s="1">
         <v>45913</v>
       </c>
-      <c r="D5" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D5" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E5" t="s">
         <v>8</v>
@@ -858,7 +866,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -868,8 +876,8 @@
       <c r="C6" s="1">
         <v>45913</v>
       </c>
-      <c r="D6" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D6" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E6" t="s">
         <v>8</v>
@@ -878,7 +886,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -888,8 +896,8 @@
       <c r="C7" s="1">
         <v>45913</v>
       </c>
-      <c r="D7" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D7" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E7" t="s">
         <v>8</v>
@@ -898,7 +906,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -908,8 +916,8 @@
       <c r="C8" s="1">
         <v>45913</v>
       </c>
-      <c r="D8" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D8" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E8" t="s">
         <v>11</v>
@@ -918,7 +926,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -928,8 +936,8 @@
       <c r="C9" s="1">
         <v>45913</v>
       </c>
-      <c r="D9" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D9" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E9" t="s">
         <v>8</v>
@@ -938,7 +946,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -948,8 +956,8 @@
       <c r="C10" s="1">
         <v>45913</v>
       </c>
-      <c r="D10" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D10" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E10" t="s">
         <v>8</v>
@@ -958,7 +966,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -968,8 +976,8 @@
       <c r="C11" s="1">
         <v>45913</v>
       </c>
-      <c r="D11" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D11" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E11" t="s">
         <v>8</v>
@@ -978,7 +986,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -988,8 +996,8 @@
       <c r="C12" s="1">
         <v>45913</v>
       </c>
-      <c r="D12" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D12" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E12" t="s">
         <v>8</v>
@@ -998,7 +1006,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -1008,8 +1016,8 @@
       <c r="C13" s="1">
         <v>45913</v>
       </c>
-      <c r="D13" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D13" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E13" t="s">
         <v>8</v>
@@ -1018,7 +1026,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -1028,8 +1036,8 @@
       <c r="C14" s="1">
         <v>45913</v>
       </c>
-      <c r="D14" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D14" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E14" t="s">
         <v>8</v>
@@ -1038,7 +1046,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -1048,8 +1056,8 @@
       <c r="C15" s="1">
         <v>45913</v>
       </c>
-      <c r="D15" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D15" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E15" t="s">
         <v>8</v>
@@ -1058,7 +1066,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -1068,8 +1076,8 @@
       <c r="C16" s="1">
         <v>45913</v>
       </c>
-      <c r="D16" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D16" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E16" t="s">
         <v>8</v>
@@ -1078,7 +1086,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -1088,8 +1096,8 @@
       <c r="C17" s="1">
         <v>45913</v>
       </c>
-      <c r="D17" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D17" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E17" t="s">
         <v>8</v>
@@ -1098,7 +1106,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -1108,8 +1116,8 @@
       <c r="C18" s="1">
         <v>45913</v>
       </c>
-      <c r="D18" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D18" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E18" t="s">
         <v>8</v>
@@ -1118,7 +1126,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -1128,8 +1136,8 @@
       <c r="C19" s="1">
         <v>45913</v>
       </c>
-      <c r="D19" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D19" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E19" t="s">
         <v>8</v>
@@ -1138,7 +1146,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -1148,8 +1156,8 @@
       <c r="C20" s="1">
         <v>45913</v>
       </c>
-      <c r="D20" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D20" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E20" t="s">
         <v>11</v>
@@ -1158,7 +1166,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -1168,8 +1176,8 @@
       <c r="C21" s="1">
         <v>45913</v>
       </c>
-      <c r="D21" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D21" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E21" t="s">
         <v>8</v>
@@ -1178,7 +1186,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -1188,8 +1196,8 @@
       <c r="C22" s="1">
         <v>45913</v>
       </c>
-      <c r="D22" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D22" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E22" t="s">
         <v>8</v>
@@ -1198,7 +1206,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -1208,8 +1216,8 @@
       <c r="C23" s="1">
         <v>45913</v>
       </c>
-      <c r="D23" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D23" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E23" t="s">
         <v>8</v>
@@ -1218,7 +1226,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -1228,8 +1236,8 @@
       <c r="C24" s="1">
         <v>45913</v>
       </c>
-      <c r="D24" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D24" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E24" t="s">
         <v>8</v>
@@ -1238,7 +1246,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -1248,8 +1256,8 @@
       <c r="C25" s="1">
         <v>45913</v>
       </c>
-      <c r="D25" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D25" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E25" t="s">
         <v>8</v>
@@ -1258,7 +1266,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -1268,8 +1276,8 @@
       <c r="C26" s="1">
         <v>45913</v>
       </c>
-      <c r="D26" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D26" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E26" t="s">
         <v>8</v>
@@ -1278,7 +1286,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -1288,8 +1296,8 @@
       <c r="C27" s="1">
         <v>45913</v>
       </c>
-      <c r="D27" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D27" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E27" t="s">
         <v>8</v>
@@ -1298,7 +1306,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -1308,8 +1316,8 @@
       <c r="C28" s="1">
         <v>45913</v>
       </c>
-      <c r="D28" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D28" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E28" t="s">
         <v>8</v>
@@ -1318,7 +1326,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>37</v>
       </c>
@@ -1328,8 +1336,8 @@
       <c r="C29" s="1">
         <v>45913</v>
       </c>
-      <c r="D29" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D29" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E29" t="s">
         <v>8</v>
@@ -1338,7 +1346,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>38</v>
       </c>
@@ -1348,8 +1356,8 @@
       <c r="C30" s="1">
         <v>45913</v>
       </c>
-      <c r="D30" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D30" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E30" t="s">
         <v>8</v>
@@ -1358,7 +1366,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>39</v>
       </c>
@@ -1368,8 +1376,8 @@
       <c r="C31" s="1">
         <v>45913</v>
       </c>
-      <c r="D31" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D31" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E31" t="s">
         <v>8</v>
@@ -1378,7 +1386,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>40</v>
       </c>
@@ -1388,8 +1396,8 @@
       <c r="C32" s="1">
         <v>45913</v>
       </c>
-      <c r="D32" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D32" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E32" t="s">
         <v>8</v>
@@ -1398,7 +1406,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>41</v>
       </c>
@@ -1408,8 +1416,8 @@
       <c r="C33" s="1">
         <v>45913</v>
       </c>
-      <c r="D33" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D33" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E33" t="s">
         <v>8</v>
@@ -1418,7 +1426,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>42</v>
       </c>
@@ -1428,8 +1436,8 @@
       <c r="C34" s="1">
         <v>45913</v>
       </c>
-      <c r="D34" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D34" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E34" t="s">
         <v>8</v>
@@ -1438,7 +1446,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>43</v>
       </c>
@@ -1448,8 +1456,8 @@
       <c r="C35" s="1">
         <v>45913</v>
       </c>
-      <c r="D35" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D35" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E35" t="s">
         <v>8</v>
@@ -1458,7 +1466,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>44</v>
       </c>
@@ -1468,8 +1476,8 @@
       <c r="C36" s="1">
         <v>45913</v>
       </c>
-      <c r="D36" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D36" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E36" t="s">
         <v>8</v>
@@ -1478,7 +1486,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>45</v>
       </c>
@@ -1488,8 +1496,8 @@
       <c r="C37" s="1">
         <v>45913</v>
       </c>
-      <c r="D37" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D37" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E37" t="s">
         <v>8</v>
@@ -1498,7 +1506,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>46</v>
       </c>
@@ -1508,8 +1516,8 @@
       <c r="C38" s="1">
         <v>45913</v>
       </c>
-      <c r="D38" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D38" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E38" t="s">
         <v>8</v>
@@ -1518,7 +1526,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>47</v>
       </c>
@@ -1528,8 +1536,8 @@
       <c r="C39" s="1">
         <v>45913</v>
       </c>
-      <c r="D39" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D39" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E39" t="s">
         <v>8</v>
@@ -1538,7 +1546,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>48</v>
       </c>
@@ -1548,8 +1556,8 @@
       <c r="C40" s="1">
         <v>45913</v>
       </c>
-      <c r="D40" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D40" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E40" t="s">
         <v>8</v>
@@ -1558,7 +1566,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>49</v>
       </c>
@@ -1568,8 +1576,8 @@
       <c r="C41" s="1">
         <v>45913</v>
       </c>
-      <c r="D41" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D41" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E41" t="s">
         <v>8</v>
@@ -1578,7 +1586,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>50</v>
       </c>
@@ -1588,8 +1596,8 @@
       <c r="C42" s="1">
         <v>45913</v>
       </c>
-      <c r="D42" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D42" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E42" t="s">
         <v>8</v>
@@ -1598,7 +1606,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>51</v>
       </c>
@@ -1608,8 +1616,8 @@
       <c r="C43" s="1">
         <v>45913</v>
       </c>
-      <c r="D43" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D43" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E43" t="s">
         <v>8</v>
@@ -1618,7 +1626,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>52</v>
       </c>
@@ -1628,8 +1636,8 @@
       <c r="C44" s="1">
         <v>45913</v>
       </c>
-      <c r="D44" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D44" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E44" t="s">
         <v>8</v>
@@ -1638,7 +1646,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>53</v>
       </c>
@@ -1648,8 +1656,8 @@
       <c r="C45" s="1">
         <v>45913</v>
       </c>
-      <c r="D45" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D45" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E45" t="s">
         <v>8</v>
@@ -1658,7 +1666,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>54</v>
       </c>
@@ -1668,8 +1676,8 @@
       <c r="C46" s="1">
         <v>45913</v>
       </c>
-      <c r="D46" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D46" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E46" t="s">
         <v>11</v>
@@ -1678,7 +1686,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>55</v>
       </c>
@@ -1688,8 +1696,8 @@
       <c r="C47" s="1">
         <v>45913</v>
       </c>
-      <c r="D47" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D47" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E47" t="s">
         <v>8</v>
@@ -1698,7 +1706,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>56</v>
       </c>
@@ -1708,8 +1716,8 @@
       <c r="C48" s="1">
         <v>45913</v>
       </c>
-      <c r="D48" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D48" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E48" t="s">
         <v>8</v>
@@ -1718,7 +1726,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>57</v>
       </c>
@@ -1728,8 +1736,8 @@
       <c r="C49" s="1">
         <v>45913</v>
       </c>
-      <c r="D49" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D49" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E49" t="s">
         <v>8</v>
@@ -1738,7 +1746,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>58</v>
       </c>
@@ -1748,8 +1756,8 @@
       <c r="C50" s="1">
         <v>45913</v>
       </c>
-      <c r="D50" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D50" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E50" t="s">
         <v>8</v>
@@ -1758,7 +1766,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>59</v>
       </c>
@@ -1768,8 +1776,8 @@
       <c r="C51" s="1">
         <v>45913</v>
       </c>
-      <c r="D51" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D51" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E51" t="s">
         <v>8</v>
@@ -1778,7 +1786,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>60</v>
       </c>
@@ -1788,8 +1796,8 @@
       <c r="C52" s="1">
         <v>45913</v>
       </c>
-      <c r="D52" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D52" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E52" t="s">
         <v>8</v>
@@ -1798,7 +1806,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>61</v>
       </c>
@@ -1808,8 +1816,8 @@
       <c r="C53" s="1">
         <v>45913</v>
       </c>
-      <c r="D53" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D53" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E53" t="s">
         <v>8</v>
@@ -1818,7 +1826,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>62</v>
       </c>
@@ -1828,8 +1836,8 @@
       <c r="C54" s="1">
         <v>45913</v>
       </c>
-      <c r="D54" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D54" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E54" t="s">
         <v>8</v>
@@ -1838,7 +1846,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>63</v>
       </c>
@@ -1848,8 +1856,8 @@
       <c r="C55" s="1">
         <v>45913</v>
       </c>
-      <c r="D55" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D55" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E55" t="s">
         <v>8</v>
@@ -1858,7 +1866,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>64</v>
       </c>
@@ -1868,8 +1876,8 @@
       <c r="C56" s="1">
         <v>45913</v>
       </c>
-      <c r="D56" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D56" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E56" t="s">
         <v>8</v>
@@ -1878,7 +1886,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>65</v>
       </c>
@@ -1888,8 +1896,8 @@
       <c r="C57" s="1">
         <v>45913</v>
       </c>
-      <c r="D57" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D57" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E57" t="s">
         <v>8</v>
@@ -1898,7 +1906,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>66</v>
       </c>
@@ -1908,8 +1916,8 @@
       <c r="C58" s="1">
         <v>45913</v>
       </c>
-      <c r="D58" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D58" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E58" t="s">
         <v>8</v>
@@ -1918,7 +1926,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>67</v>
       </c>
@@ -1928,8 +1936,8 @@
       <c r="C59" s="1">
         <v>45913</v>
       </c>
-      <c r="D59" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D59" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E59" t="s">
         <v>8</v>
@@ -1938,7 +1946,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>68</v>
       </c>
@@ -1948,8 +1956,8 @@
       <c r="C60" s="1">
         <v>45913</v>
       </c>
-      <c r="D60" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D60" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E60" t="s">
         <v>8</v>
@@ -1958,7 +1966,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>69</v>
       </c>
@@ -1968,8 +1976,8 @@
       <c r="C61" s="1">
         <v>45913</v>
       </c>
-      <c r="D61" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D61" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E61" t="s">
         <v>11</v>
@@ -1978,7 +1986,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>70</v>
       </c>
@@ -1988,8 +1996,8 @@
       <c r="C62" s="1">
         <v>45913</v>
       </c>
-      <c r="D62" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D62" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E62" t="s">
         <v>8</v>
@@ -1998,7 +2006,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>71</v>
       </c>
@@ -2008,8 +2016,8 @@
       <c r="C63" s="1">
         <v>45913</v>
       </c>
-      <c r="D63" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D63" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E63" t="s">
         <v>8</v>
@@ -2018,7 +2026,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>72</v>
       </c>
@@ -2028,8 +2036,8 @@
       <c r="C64" s="1">
         <v>45913</v>
       </c>
-      <c r="D64" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D64" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E64" t="s">
         <v>8</v>
@@ -2038,7 +2046,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>73</v>
       </c>
@@ -2048,8 +2056,8 @@
       <c r="C65" s="1">
         <v>45913</v>
       </c>
-      <c r="D65" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D65" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E65" t="s">
         <v>8</v>
@@ -2058,7 +2066,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>74</v>
       </c>
@@ -2068,8 +2076,8 @@
       <c r="C66" s="1">
         <v>45913</v>
       </c>
-      <c r="D66" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D66" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E66" t="s">
         <v>8</v>
@@ -2078,7 +2086,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>75</v>
       </c>
@@ -2088,8 +2096,8 @@
       <c r="C67" s="1">
         <v>45913</v>
       </c>
-      <c r="D67" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D67" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E67" t="s">
         <v>8</v>
@@ -2098,7 +2106,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>76</v>
       </c>
@@ -2108,8 +2116,8 @@
       <c r="C68" s="1">
         <v>45913</v>
       </c>
-      <c r="D68" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D68" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E68" t="s">
         <v>8</v>
@@ -2118,7 +2126,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>77</v>
       </c>
@@ -2128,8 +2136,8 @@
       <c r="C69" s="1">
         <v>45913</v>
       </c>
-      <c r="D69" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D69" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E69" t="s">
         <v>8</v>
@@ -2138,7 +2146,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>78</v>
       </c>
@@ -2148,8 +2156,8 @@
       <c r="C70" s="1">
         <v>45913</v>
       </c>
-      <c r="D70" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D70" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E70" t="s">
         <v>8</v>
@@ -2158,7 +2166,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>79</v>
       </c>
@@ -2168,8 +2176,8 @@
       <c r="C71" s="1">
         <v>45913</v>
       </c>
-      <c r="D71" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D71" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E71" t="s">
         <v>11</v>
@@ -2178,7 +2186,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>80</v>
       </c>
@@ -2188,8 +2196,8 @@
       <c r="C72" s="1">
         <v>45913</v>
       </c>
-      <c r="D72" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D72" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E72" t="s">
         <v>11</v>
@@ -2198,7 +2206,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>81</v>
       </c>
@@ -2208,8 +2216,8 @@
       <c r="C73" s="1">
         <v>45913</v>
       </c>
-      <c r="D73" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D73" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E73" t="s">
         <v>8</v>
@@ -2218,7 +2226,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>82</v>
       </c>
@@ -2228,8 +2236,8 @@
       <c r="C74" s="1">
         <v>45913</v>
       </c>
-      <c r="D74" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D74" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E74" t="s">
         <v>8</v>
@@ -2238,7 +2246,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>83</v>
       </c>
@@ -2248,8 +2256,8 @@
       <c r="C75" s="1">
         <v>45913</v>
       </c>
-      <c r="D75" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D75" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E75" t="s">
         <v>8</v>
@@ -2258,7 +2266,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>84</v>
       </c>
@@ -2268,8 +2276,8 @@
       <c r="C76" s="1">
         <v>45913</v>
       </c>
-      <c r="D76" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D76" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E76" t="s">
         <v>8</v>
@@ -2278,7 +2286,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>85</v>
       </c>
@@ -2288,8 +2296,8 @@
       <c r="C77" s="1">
         <v>45913</v>
       </c>
-      <c r="D77" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D77" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E77" t="s">
         <v>8</v>
@@ -2298,7 +2306,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>86</v>
       </c>
@@ -2308,8 +2316,8 @@
       <c r="C78" s="1">
         <v>45913</v>
       </c>
-      <c r="D78" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D78" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E78" t="s">
         <v>8</v>
@@ -2318,7 +2326,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>87</v>
       </c>
@@ -2328,8 +2336,8 @@
       <c r="C79" s="1">
         <v>45913</v>
       </c>
-      <c r="D79" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D79" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E79" t="s">
         <v>8</v>
@@ -2338,7 +2346,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>88</v>
       </c>
@@ -2348,8 +2356,8 @@
       <c r="C80" s="1">
         <v>45913</v>
       </c>
-      <c r="D80" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D80" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E80" t="s">
         <v>8</v>
@@ -2358,7 +2366,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>89</v>
       </c>
@@ -2368,8 +2376,8 @@
       <c r="C81" s="1">
         <v>45913</v>
       </c>
-      <c r="D81" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D81" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E81" t="s">
         <v>8</v>
@@ -2378,7 +2386,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>90</v>
       </c>
@@ -2388,8 +2396,8 @@
       <c r="C82" s="1">
         <v>45913</v>
       </c>
-      <c r="D82" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D82" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E82" t="s">
         <v>8</v>
@@ -2398,7 +2406,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>91</v>
       </c>
@@ -2408,8 +2416,8 @@
       <c r="C83" s="1">
         <v>45913</v>
       </c>
-      <c r="D83" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D83" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E83" t="s">
         <v>11</v>
@@ -2418,7 +2426,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>92</v>
       </c>
@@ -2428,8 +2436,8 @@
       <c r="C84" s="1">
         <v>45913</v>
       </c>
-      <c r="D84" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D84" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E84" t="s">
         <v>11</v>
@@ -2438,7 +2446,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>93</v>
       </c>
@@ -2448,8 +2456,8 @@
       <c r="C85" s="1">
         <v>45913</v>
       </c>
-      <c r="D85" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D85" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E85" t="s">
         <v>8</v>
@@ -2458,7 +2466,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>94</v>
       </c>
@@ -2468,8 +2476,8 @@
       <c r="C86" s="1">
         <v>45913</v>
       </c>
-      <c r="D86" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D86" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E86" t="s">
         <v>8</v>
@@ -2478,7 +2486,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>95</v>
       </c>
@@ -2488,8 +2496,8 @@
       <c r="C87" s="1">
         <v>45913</v>
       </c>
-      <c r="D87" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D87" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E87" t="s">
         <v>8</v>
@@ -2498,7 +2506,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>96</v>
       </c>
@@ -2508,8 +2516,8 @@
       <c r="C88" s="1">
         <v>45913</v>
       </c>
-      <c r="D88" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D88" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E88" t="s">
         <v>8</v>
@@ -2518,7 +2526,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>97</v>
       </c>
@@ -2528,8 +2536,8 @@
       <c r="C89" s="1">
         <v>45913</v>
       </c>
-      <c r="D89" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D89" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E89" t="s">
         <v>11</v>
@@ -2538,7 +2546,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>98</v>
       </c>
@@ -2548,8 +2556,8 @@
       <c r="C90" s="1">
         <v>45913</v>
       </c>
-      <c r="D90" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D90" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E90" t="s">
         <v>8</v>
@@ -2558,7 +2566,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>99</v>
       </c>
@@ -2568,8 +2576,8 @@
       <c r="C91" s="1">
         <v>45913</v>
       </c>
-      <c r="D91" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D91" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E91" t="s">
         <v>8</v>
@@ -2578,7 +2586,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>100</v>
       </c>
@@ -2588,8 +2596,8 @@
       <c r="C92" s="1">
         <v>45913</v>
       </c>
-      <c r="D92" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D92" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E92" t="s">
         <v>8</v>
@@ -2598,7 +2606,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>101</v>
       </c>
@@ -2608,8 +2616,8 @@
       <c r="C93" s="1">
         <v>45913</v>
       </c>
-      <c r="D93" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D93" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E93" t="s">
         <v>8</v>
@@ -2618,7 +2626,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>102</v>
       </c>
@@ -2628,8 +2636,8 @@
       <c r="C94" s="1">
         <v>45913</v>
       </c>
-      <c r="D94" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D94" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E94" t="s">
         <v>8</v>
@@ -2638,7 +2646,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>103</v>
       </c>
@@ -2648,8 +2656,8 @@
       <c r="C95" s="1">
         <v>45913</v>
       </c>
-      <c r="D95" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D95" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E95" t="s">
         <v>8</v>
@@ -2658,7 +2666,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>104</v>
       </c>
@@ -2668,8 +2676,8 @@
       <c r="C96" s="1">
         <v>45913</v>
       </c>
-      <c r="D96" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D96" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E96" t="s">
         <v>8</v>
@@ -2678,7 +2686,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>105</v>
       </c>
@@ -2688,8 +2696,8 @@
       <c r="C97" s="1">
         <v>45913</v>
       </c>
-      <c r="D97" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D97" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E97" t="s">
         <v>8</v>
@@ -2698,7 +2706,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="98" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>106</v>
       </c>
@@ -2708,8 +2716,8 @@
       <c r="C98" s="1">
         <v>45913</v>
       </c>
-      <c r="D98" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D98" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E98" t="s">
         <v>11</v>
@@ -2718,7 +2726,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>107</v>
       </c>
@@ -2728,8 +2736,8 @@
       <c r="C99" s="1">
         <v>45913</v>
       </c>
-      <c r="D99" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D99" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E99" t="s">
         <v>8</v>
@@ -2738,7 +2746,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>108</v>
       </c>
@@ -2748,8 +2756,8 @@
       <c r="C100" s="1">
         <v>45913</v>
       </c>
-      <c r="D100" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D100" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E100" t="s">
         <v>8</v>
@@ -2758,7 +2766,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="101" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>109</v>
       </c>
@@ -2768,8 +2776,8 @@
       <c r="C101" s="1">
         <v>45913</v>
       </c>
-      <c r="D101" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D101" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E101" t="s">
         <v>8</v>
@@ -2778,7 +2786,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>110</v>
       </c>
@@ -2788,8 +2796,8 @@
       <c r="C102" s="1">
         <v>45913</v>
       </c>
-      <c r="D102" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D102" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E102" t="s">
         <v>8</v>
@@ -2798,7 +2806,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="103" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>111</v>
       </c>
@@ -2808,8 +2816,8 @@
       <c r="C103" s="1">
         <v>45913</v>
       </c>
-      <c r="D103" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D103" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E103" t="s">
         <v>11</v>
@@ -2818,7 +2826,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="104" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>112</v>
       </c>
@@ -2828,8 +2836,8 @@
       <c r="C104" s="1">
         <v>45913</v>
       </c>
-      <c r="D104" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D104" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E104" t="s">
         <v>8</v>
@@ -2838,7 +2846,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="105" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>113</v>
       </c>
@@ -2848,8 +2856,8 @@
       <c r="C105" s="1">
         <v>45913</v>
       </c>
-      <c r="D105" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D105" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E105" t="s">
         <v>8</v>
@@ -2858,7 +2866,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="106" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>114</v>
       </c>
@@ -2868,8 +2876,8 @@
       <c r="C106" s="1">
         <v>45913</v>
       </c>
-      <c r="D106" s="2">
-        <v>0.48622685185185183</v>
+      <c r="D106" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E106" t="s">
         <v>11</v>

</xml_diff>